<commit_message>
Checkpoint before assistant change: Update user interaction flow to verify channel subscription status
Implement subscription verification before proceeding with bot operations.

Replit-Commit-Author: Assistant
</commit_message>
<xml_diff>
--- a/replit_postgres_bot/история.xlsx
+++ b/replit_postgres_bot/история.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -493,6 +493,36 @@
         <v>42200</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2025-06-28 05:31</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Роман Тарифы FSTA</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>600</v>
+      </c>
+      <c r="D3" t="n">
+        <v>200</v>
+      </c>
+      <c r="E3" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F3" t="n">
+        <v>24</v>
+      </c>
+      <c r="G3" t="n">
+        <v>5</v>
+      </c>
+      <c r="H3" t="n">
+        <v>7600</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>